<commit_message>
refactor: excel code is modified
</commit_message>
<xml_diff>
--- a/storage/Template/Excel/Ordenes_servicio.xlsx
+++ b/storage/Template/Excel/Ordenes_servicio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Prisma\Prisma-PHP\storage\Template\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santiago2730\Documents\proyectos\prisma\prisma-php\storage\Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F898F5D6-3AA9-460A-B4D0-80F24EC492CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824C51B3-3528-44B7-A5B3-533225CB93BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,46 +38,46 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>ESTADO DEL SERVICIO</t>
-  </si>
-  <si>
-    <t>NOMBRE COMPLETO PROVEDOR</t>
-  </si>
-  <si>
-    <t>IDPRODUCTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FECHA DE CREACION </t>
-  </si>
-  <si>
-    <t>FECHA DE  ENTREGA</t>
-  </si>
-  <si>
-    <t>PRODUCTO TRANSFORMADO</t>
-  </si>
-  <si>
-    <t>TIPO DE ORDEN</t>
-  </si>
-  <si>
     <t>CONSECUTIVO</t>
   </si>
   <si>
-    <t>CANTIDAD PRODUCTO</t>
-  </si>
-  <si>
-    <t>CANTIDAD DEFECTUOSAS</t>
-  </si>
-  <si>
     <t>CANTIDAD BUENAS</t>
   </si>
   <si>
     <t>CANTIDAD PENDIENTES</t>
   </si>
   <si>
-    <t>OBSERVACIONES</t>
-  </si>
-  <si>
-    <t>TOTAL PRECIO</t>
+    <t>ESTADO  DE ORDEN DE SERVICIO</t>
+  </si>
+  <si>
+    <t>PRODUCTO</t>
+  </si>
+  <si>
+    <t>PROVEDOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIPO DE ORDEN </t>
+  </si>
+  <si>
+    <t>CANTIDAD PRODUCTOS</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>PRODUCTO FINAL</t>
+  </si>
+  <si>
+    <t>FECHA DE CREACIÓN</t>
+  </si>
+  <si>
+    <t>FECHA DE ENTREGA</t>
+  </si>
+  <si>
+    <t>CANTIDAD MALAS</t>
+  </si>
+  <si>
+    <t>OBSERVACIÓN</t>
   </si>
 </sst>
 </file>
@@ -141,7 +141,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -151,6 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -200,16 +200,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>857250</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1981200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>139073</xdr:rowOff>
+      <xdr:rowOff>129548</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -238,7 +238,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13820775" y="57151"/>
+          <a:off x="12896850" y="47626"/>
           <a:ext cx="2286000" cy="462922"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -255,20 +255,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A5:N6" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A5:N6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ESTADO DEL SERVICIO"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE COMPLETO PROVEDOR"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="IDPRODUCTO"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FECHA DE CREACION "/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="FECHA DE  ENTREGA"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PRODUCTO TRANSFORMADO"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="TIPO DE ORDEN"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="CONSECUTIVO"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="CANTIDAD PRODUCTO"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CANTIDAD BUENAS"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="CANTIDAD DEFECTUOSAS"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="CANTIDAD PENDIENTES"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="OBSERVACIONES"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="TOTAL PRECIO"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CONSECUTIVO"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTADO  DE ORDEN DE SERVICIO"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PRODUCTO"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TIPO DE ORDEN "/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="PROVEDOR"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="CANTIDAD PRODUCTOS"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="PRECIO"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PRODUCTO FINAL"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA DE CREACIÓN"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="FECHA DE ENTREGA"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="CANTIDAD MALAS"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="CANTIDAD BUENAS"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="CANTIDAD PENDIENTES"/>
+    <tableColumn id="13" xr3:uid="{69CD743D-62B3-4DB8-86B1-FB4800610DE6}" name="OBSERVACIÓN"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -571,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,62 +586,60 @@
     <col min="8" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="10" width="31.140625" customWidth="1"/>
     <col min="11" max="11" width="31.42578125" customWidth="1"/>
-    <col min="12" max="14" width="30.7109375" customWidth="1"/>
+    <col min="12" max="13" width="30.7109375" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="1"/>
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="1"/>
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="1"/>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -656,47 +654,47 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="M5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
style: excel template has been updated
</commit_message>
<xml_diff>
--- a/storage/Template/Excel/Ordenes_servicio.xlsx
+++ b/storage/Template/Excel/Ordenes_servicio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santiago2730\Documents\proyectos\prisma\prisma-php\storage\Template\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\Projects\prisma\prisma-php\storage\Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824C51B3-3528-44B7-A5B3-533225CB93BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E9449F-D285-44C3-9CE2-E9634E64DB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ORDENES_SERVICIO" sheetId="1" r:id="rId1"/>
@@ -147,10 +147,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,72 +587,72 @@
     <col min="9" max="10" width="31.140625" customWidth="1"/>
     <col min="11" max="11" width="31.42578125" customWidth="1"/>
     <col min="12" max="13" width="30.7109375" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
ci: excel export has been modified
</commit_message>
<xml_diff>
--- a/storage/Template/Excel/Ordenes_servicio.xlsx
+++ b/storage/Template/Excel/Ordenes_servicio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\Projects\prisma\prisma-php\storage\Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E9449F-D285-44C3-9CE2-E9634E64DB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55657470-2162-4645-BA10-B39231E349A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CONSECUTIVO</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>OBSERVACIÓN</t>
+  </si>
+  <si>
+    <t>CANTIDAD TOTAL</t>
   </si>
 </sst>
 </file>
@@ -252,9 +255,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A5:N6" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A5:N6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A5:O6" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A5:O6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CONSECUTIVO"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTADO  DE ORDEN DE SERVICIO"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PRODUCTO"/>
@@ -265,6 +268,7 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PRODUCTO FINAL"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA DE CREACIÓN"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="FECHA DE ENTREGA"/>
+    <tableColumn id="15" xr3:uid="{C2EB26B2-B645-432D-BDBF-F4FA10C5C61D}" name="CANTIDAD TOTAL"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="CANTIDAD MALAS"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="CANTIDAD BUENAS"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="CANTIDAD PENDIENTES"/>
@@ -571,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,13 +588,13 @@
     <col min="3" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="10" width="31.140625" customWidth="1"/>
-    <col min="11" max="11" width="31.42578125" customWidth="1"/>
-    <col min="12" max="13" width="30.7109375" customWidth="1"/>
-    <col min="14" max="14" width="50.7109375" customWidth="1"/>
+    <col min="9" max="11" width="31.140625" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" customWidth="1"/>
+    <col min="13" max="14" width="30.7109375" customWidth="1"/>
+    <col min="15" max="15" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -605,8 +609,9 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -621,8 +626,9 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -637,8 +643,9 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -653,8 +660,9 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,22 +694,25 @@
         <v>11</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:N3"/>
-    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A1:O3"/>
+    <mergeCell ref="A4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ci: excel have been modified
</commit_message>
<xml_diff>
--- a/storage/Template/Excel/Ordenes_servicio.xlsx
+++ b/storage/Template/Excel/Ordenes_servicio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\Projects\prisma\prisma-php\storage\Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55657470-2162-4645-BA10-B39231E349A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CCA5B9-BC38-4632-BC1E-03470EE89C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,13 +204,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1981200</xdr:colOff>
+      <xdr:colOff>1965614</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>123826</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>129548</xdr:rowOff>
     </xdr:to>
@@ -241,8 +241,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12896850" y="47626"/>
-          <a:ext cx="2286000" cy="462922"/>
+          <a:off x="12902046" y="47626"/>
+          <a:ext cx="2305916" cy="462922"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refactor: models were organized
</commit_message>
<xml_diff>
--- a/storage/Template/Excel/Ordenes_servicio.xlsx
+++ b/storage/Template/Excel/Ordenes_servicio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\Projects\prisma\prisma-php\storage\Template\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santiago2730\Documents\proyectos\prisma\prisma-php\storage\Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CCA5B9-BC38-4632-BC1E-03470EE89C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07EDB3-EFE5-46DA-8AE9-998251FEB6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21636" yWindow="2244" windowWidth="15372" windowHeight="7872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ORDENES_SERVICIO" sheetId="1" r:id="rId1"/>

</xml_diff>